<commit_message>
重命名了baseline的文件名，记录double dqn + reduce world pool 的结果分析
</commit_message>
<xml_diff>
--- a/实验记录.xlsx
+++ b/实验记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_repo\DDQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1602778B-787D-44E0-8D4B-AEE488A17703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165AFDE4-6037-427D-AD01-8927B2E4AD23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D358A1CB-436A-4388-BFF8-0C41C401868E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>实验结果路径</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -67,117 +67,122 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>4，planing时与user交互而不是与world model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseline_ddq_k5_5_agent_800_epoches</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>improve_td_err-newly_experience</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>improve-newly_experience</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>利用经验池中哪些经验训练agent，5000大小的池，默认全部</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2021.6.6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>improve-newly_experience-pool_5000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>train_on_experience_for_more_epoches</t>
+  </si>
+  <si>
+    <t>2021.6.7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce_world_pool</t>
+  </si>
+  <si>
+    <t>agent对经验池的训练epochs，默认1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>agent经验池大小，默认world/user pool都是5000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>world pool 1500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>结论：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 对agent的每个经验训练3次不如每个经验训练1次</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 减小world model 经验池会提高模型性能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce_world_pool-td_err_sample</t>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>double_dqn</t>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否将底层DQN改为Double DQN，默认否</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.设置replay pool(world model)大小为1500时，使用td-err双倍采样再取单倍样本使训练波动更大，效果只设置reply pool更差</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.double_ddq在前期有一点点效果，后期反而使效果降低了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>double_dqn-reduce_pool</t>
+  </si>
+  <si>
+    <t>world pool 1500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>猜想： double dqn 与 reduce pool一起作用的效果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>baseline_dqn_k5_5_agent_800_epoches</t>
-  </si>
-  <si>
-    <t>4，planing时与user交互而不是与world model</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>baseline_ddq_k5_5_agent_800_epoches</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>improve_td_err-newly_experience</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>improve-newly_experience</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>利用经验池中哪些经验训练agent，5000大小的池，默认全部</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2021.6.6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>improve-newly_experience-pool_5000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>train_on_experience_for_more_epoches</t>
-  </si>
-  <si>
-    <t>2021.6.7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce_world_pool</t>
-  </si>
-  <si>
-    <t>agent对经验池的训练epochs，默认1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>agent经验池大小，默认world/user pool都是5000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>world pool 1500</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>结论：</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. 对agent的每个经验训练3次不如每个经验训练1次</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. 减小world model 经验池会提高模型性能</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce_world_pool-td_err_sample</t>
-  </si>
-  <si>
-    <t>是</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6.10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>double_dqn</t>
-  </si>
-  <si>
-    <t>是</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是否将底层DQN改为Double DQN，默认否</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6.11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.设置replay pool(world model)大小为1500时，使用td-err双倍采样再取单倍样本使训练波动更大，效果只设置reply pool更差</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.double_ddq在前期有一点点效果，后期反而使效果降低了</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>double_dqn-reduce_pool</t>
-  </si>
-  <si>
-    <t>world pool 1500</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>猜想： double dqn 与 reduce pool一起作用的效果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. double_ddq结合reduce_world_pool 效果比单独的reduce_world_pool好一点点</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -185,7 +190,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,14 +211,6 @@
       <color rgb="FFFF0000"/>
       <name val="等线"/>
       <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -248,7 +245,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -261,28 +258,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -599,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD510B64-0C2A-47AE-A5B9-9ADFAE468889}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -615,7 +603,7 @@
     <col min="6" max="6" width="13" style="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="2"/>
     <col min="8" max="8" width="9" style="1"/>
-    <col min="10" max="10" width="9" style="5"/>
+    <col min="10" max="10" width="9" style="4"/>
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -636,16 +624,16 @@
         <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
@@ -653,7 +641,7 @@
     </row>
     <row r="2" spans="1:10" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1">
         <v>400</v>
@@ -670,13 +658,13 @@
       <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1">
         <v>400</v>
@@ -690,13 +678,13 @@
       <c r="H3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1">
         <v>800</v>
@@ -707,13 +695,13 @@
       <c r="D5" s="1">
         <v>4</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="B6" s="1">
         <v>800</v>
@@ -722,15 +710,15 @@
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1">
         <v>400</v>
@@ -742,15 +730,15 @@
         <v>4</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1">
         <v>400</v>
@@ -762,129 +750,137 @@
         <v>4</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J8" s="5">
+        <v>23</v>
+      </c>
+      <c r="J8" s="4">
         <v>6.7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="7" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:10" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="5">
+        <v>400</v>
+      </c>
+      <c r="C9" s="5">
+        <v>3</v>
+      </c>
+      <c r="D9" s="5">
+        <v>4</v>
+      </c>
+      <c r="F9" s="5">
+        <v>3</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="J9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="7">
+    </row>
+    <row r="10" spans="1:10" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="5">
         <v>400</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C10" s="5">
         <v>3</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D10" s="5">
         <v>4</v>
       </c>
-      <c r="F9" s="7">
+      <c r="E10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="8"/>
+      <c r="J10" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="5">
+        <v>400</v>
+      </c>
+      <c r="C11" s="5">
         <v>3</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="J9" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="7" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="7">
+      <c r="D11" s="5">
+        <v>4</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="I11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="5">
         <v>400</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C12" s="5">
         <v>3</v>
       </c>
-      <c r="D10" s="7">
-        <v>4</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" s="11"/>
-      <c r="J10" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="D12" s="5">
+        <v>3</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="7">
-        <v>400</v>
-      </c>
-      <c r="C11" s="7">
-        <v>3</v>
-      </c>
-      <c r="D11" s="7">
-        <v>4</v>
-      </c>
-      <c r="G11" s="8"/>
-      <c r="I11" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="3">
-        <v>400</v>
-      </c>
-      <c r="C12" s="3">
-        <v>3</v>
-      </c>
-      <c r="D12" s="3">
-        <v>3</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>34</v>
+      <c r="J12" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="57" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>